<commit_message>
file download is working now
</commit_message>
<xml_diff>
--- a/backend/temp_results.xlsx
+++ b/backend/temp_results.xlsx
@@ -6614,19 +6614,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.7857142857142857</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E2">
-        <v>0.8421052631578947</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F2">
-        <v>0.9285714285714285</v>
+        <v>0.9474747474747475</v>
       </c>
       <c r="G2">
-        <v>0.8759398496240601</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6637,19 +6637,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D3">
-        <v>0.3333333333333333</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E3">
-        <v>0.8421052631578947</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F3">
-        <v>0.7777777777777778</v>
+        <v>0.9474747474747475</v>
       </c>
       <c r="G3">
-        <v>0.8421052631578947</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6660,19 +6660,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.88</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E4">
-        <v>0.8421052631578947</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F4">
-        <v>0.7933333333333333</v>
+        <v>0.9474747474747475</v>
       </c>
       <c r="G4">
-        <v>0.8121052631578948</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6680,16 +6680,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.8421052631578947</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F5">
         <v>38</v>
@@ -6739,19 +6739,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D2">
-        <v>0.75</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E2">
-        <v>0.9210526315789473</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F2">
-        <v>0.9166666666666666</v>
+        <v>0.9474747474747475</v>
       </c>
       <c r="G2">
-        <v>0.9407894736842105</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6762,19 +6762,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.8636363636363636</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E3">
-        <v>0.9210526315789473</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F3">
-        <v>0.9545454545454546</v>
+        <v>0.9474747474747475</v>
       </c>
       <c r="G3">
-        <v>0.9210526315789473</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6785,19 +6785,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9268292682926829</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D4">
-        <v>0.8571428571428571</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E4">
-        <v>0.9210526315789473</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F4">
-        <v>0.9279907084785134</v>
+        <v>0.9474747474747475</v>
       </c>
       <c r="G4">
-        <v>0.9238034109664405</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6805,16 +6805,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.9210526315789473</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="F5">
         <v>38</v>
@@ -6867,16 +6867,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.75</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="E2">
-        <v>0.9210526315789473</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="F2">
-        <v>0.9166666666666666</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="G2">
-        <v>0.9407894736842105</v>
+        <v>0.975877192982456</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6887,19 +6887,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.8636363636363636</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.9210526315789473</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="F3">
-        <v>0.9545454545454546</v>
+        <v>0.9777777777777779</v>
       </c>
       <c r="G3">
-        <v>0.9210526315789473</v>
+        <v>0.9736842105263158</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6910,19 +6910,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9268292682926829</v>
+        <v>0.9655172413793104</v>
       </c>
       <c r="D4">
-        <v>0.8571428571428571</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="E4">
-        <v>0.9210526315789473</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="F4">
-        <v>0.9279907084785134</v>
+        <v>0.9740129935032483</v>
       </c>
       <c r="G4">
-        <v>0.9238034109664405</v>
+        <v>0.9738025723980116</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6930,16 +6930,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.9210526315789473</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="F5">
         <v>38</v>
@@ -6989,19 +6989,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.9</v>
+        <v>0.4230769230769231</v>
       </c>
       <c r="E2">
-        <v>0.9736842105263158</v>
+        <v>0.6052631578947368</v>
       </c>
       <c r="F2">
-        <v>0.9666666666666667</v>
+        <v>0.4743589743589744</v>
       </c>
       <c r="G2">
-        <v>0.9763157894736842</v>
+        <v>0.4382591093117409</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7012,19 +7012,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9545454545454546</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.9736842105263158</v>
+        <v>0.6052631578947368</v>
       </c>
       <c r="F3">
-        <v>0.9848484848484849</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G3">
-        <v>0.9736842105263158</v>
+        <v>0.6052631578947368</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7035,19 +7035,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9767441860465117</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.9473684210526316</v>
+        <v>0.5945945945945945</v>
       </c>
       <c r="E4">
-        <v>0.9736842105263158</v>
+        <v>0.6052631578947368</v>
       </c>
       <c r="F4">
-        <v>0.9747042023663811</v>
+        <v>0.5315315315315315</v>
       </c>
       <c r="G4">
-        <v>0.9740707337499196</v>
+        <v>0.4879089615931721</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7055,16 +7055,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.9736842105263158</v>
+        <v>0.6052631578947368</v>
       </c>
       <c r="F5">
         <v>38</v>

</xml_diff>

<commit_message>
Data Cleaning and model done
</commit_message>
<xml_diff>
--- a/backend/temp_results.xlsx
+++ b/backend/temp_results.xlsx
@@ -6611,22 +6611,22 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.7058823529411765</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="C2">
+        <v>0.625</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0.8823529411764706</v>
-      </c>
       <c r="E2">
-        <v>0.8157894736842105</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="F2">
-        <v>0.8627450980392157</v>
+        <v>0.7283333333333334</v>
       </c>
       <c r="G2">
-        <v>0.8606811145510835</v>
+        <v>0.7293421052631579</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6637,19 +6637,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.3636363636363636</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="E3">
-        <v>0.8157894736842105</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="F3">
-        <v>0.787878787878788</v>
+        <v>0.6130536130536131</v>
       </c>
       <c r="G3">
-        <v>0.8157894736842105</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6657,22 +6657,22 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.8275862068965517</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="C4">
-        <v>0.5333333333333333</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="D4">
-        <v>0.9375</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E4">
-        <v>0.8157894736842105</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="F4">
-        <v>0.7661398467432949</v>
+        <v>0.5999400209926525</v>
       </c>
       <c r="G4">
-        <v>0.7857947670901391</v>
+        <v>0.6069204725714421</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6680,16 +6680,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>0.8157894736842105</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="F5">
         <v>38</v>
@@ -6742,16 +6742,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.8823529411764706</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.9607843137254902</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0.9535603715170279</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6762,19 +6762,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.8181818181818182</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.9393939393939394</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6785,19 +6785,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.9375</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0.9458333333333333</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0.9463815789473684</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6805,16 +6805,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>38</v>
@@ -6867,16 +6867,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.9375</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E2">
         <v>0.9736842105263158</v>
       </c>
       <c r="F2">
-        <v>0.9791666666666666</v>
+        <v>0.9761904761904763</v>
       </c>
       <c r="G2">
-        <v>0.975328947368421</v>
+        <v>0.9755639097744361</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6913,16 +6913,16 @@
         <v>0.9523809523809523</v>
       </c>
       <c r="D4">
-        <v>0.967741935483871</v>
+        <v>0.962962962962963</v>
       </c>
       <c r="E4">
         <v>0.9736842105263158</v>
       </c>
       <c r="F4">
-        <v>0.9733742959549412</v>
+        <v>0.9717813051146384</v>
       </c>
       <c r="G4">
-        <v>0.9734820923275931</v>
+        <v>0.9735449735449735</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6930,13 +6930,13 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>0.9736842105263158</v>
@@ -6992,16 +6992,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.9375</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.9736842105263158</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.9791666666666666</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0.975328947368421</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7012,19 +7012,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9090909090909091</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.9736842105263158</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.9696969696969697</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9736842105263158</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7035,19 +7035,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9523809523809523</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.967741935483871</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.9736842105263158</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0.9733742959549412</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0.9734820923275931</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7055,16 +7055,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>0.9736842105263158</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>38</v>

</xml_diff>